<commit_message>
Handling boxes in digital inventory form
</commit_message>
<xml_diff>
--- a/public/excel/digital_inventory_template.xlsx
+++ b/public/excel/digital_inventory_template.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">UPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
   </si>
   <si>
     <t xml:space="preserve">serial</t>
@@ -142,13 +145,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -166,6 +169,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>